<commit_message>
Added JSON and such, Form Calculator is not working, due to line 6?
</commit_message>
<xml_diff>
--- a/data/location.xlsx
+++ b/data/location.xlsx
@@ -19,36 +19,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="748" uniqueCount="382">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="374">
   <si>
     <t>VALUE</t>
   </si>
   <si>
     <t>LOCATION</t>
-  </si>
-  <si>
-    <t>CRAIGIE 6025</t>
-  </si>
-  <si>
-    <t>CRAWLEY 6009</t>
-  </si>
-  <si>
-    <t>CULLACABARDEE 6067</t>
-  </si>
-  <si>
-    <t>CURRAMBINE 6028</t>
-  </si>
-  <si>
-    <t>DAGLISH 6008</t>
-  </si>
-  <si>
-    <t>DALKEITH 6009</t>
-  </si>
-  <si>
-    <t>DARCH 6065</t>
-  </si>
-  <si>
-    <t>DARLING DOWNS 6122</t>
   </si>
   <si>
     <t>POSTCODE</t>
@@ -1525,8 +1501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C372"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
-      <selection activeCell="B84" sqref="B84"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A364" sqref="A364"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1544,2972 +1520,4085 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C2">
         <v>6064</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C3">
         <v>6154</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C4">
         <v>6038</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C5">
         <v>6167</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="C6">
         <v>6153</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C7">
         <v>6153</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C8">
         <v>6112</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C9">
         <v>6104</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C10">
         <v>6065</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C11">
         <v>6054</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C12">
         <v>6156</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
       <c r="B13" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C13">
         <v>6164</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12</v>
+      </c>
       <c r="B14" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C14">
         <v>6164</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>13</v>
+      </c>
       <c r="B15" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C15">
         <v>6069</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>14</v>
+      </c>
       <c r="B16" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="C16">
         <v>6021</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>15</v>
+      </c>
       <c r="B17" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C17">
         <v>6171</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>16</v>
+      </c>
       <c r="B18" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="C18">
         <v>6061</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>17</v>
+      </c>
       <c r="B19" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="C19">
         <v>6066</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>18</v>
+      </c>
       <c r="B20" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="C20">
         <v>6164</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>19</v>
+      </c>
       <c r="B21" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="C21">
         <v>6031</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>20</v>
+      </c>
       <c r="B22" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C22">
         <v>6209</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>21</v>
+      </c>
       <c r="B23" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="C23">
         <v>6056</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>22</v>
+      </c>
       <c r="B24" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C24">
         <v>6054</v>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>23</v>
+      </c>
       <c r="B25" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="C25">
         <v>6150</v>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>24</v>
+      </c>
       <c r="B26" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="C26">
         <v>6053</v>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>25</v>
+      </c>
       <c r="B27" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C27">
         <v>6162</v>
       </c>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>26</v>
+      </c>
       <c r="B28" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="C28">
         <v>6107</v>
       </c>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>27</v>
+      </c>
       <c r="B29" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="C29">
         <v>6052</v>
       </c>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>28</v>
+      </c>
       <c r="B30" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="C30">
         <v>6112</v>
       </c>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>29</v>
+      </c>
       <c r="B31" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="C31">
         <v>6063</v>
       </c>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>30</v>
+      </c>
       <c r="B32" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="C32">
         <v>6556</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>31</v>
+      </c>
       <c r="B33" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="C33">
         <v>6164</v>
       </c>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>32</v>
+      </c>
       <c r="B34" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="C34">
         <v>6027</v>
       </c>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>33</v>
+      </c>
       <c r="B35" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="C35">
         <v>6069</v>
       </c>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>34</v>
+      </c>
       <c r="B36" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C36">
         <v>6056</v>
       </c>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>35</v>
+      </c>
       <c r="B37" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="C37">
         <v>6104</v>
       </c>
     </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>36</v>
+      </c>
       <c r="B38" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C38">
         <v>6063</v>
       </c>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>37</v>
+      </c>
       <c r="B39" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C39">
         <v>6102</v>
       </c>
     </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>38</v>
+      </c>
       <c r="B40" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="C40">
         <v>6167</v>
       </c>
     </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>39</v>
+      </c>
       <c r="B41" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="C41">
         <v>6163</v>
       </c>
     </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>40</v>
+      </c>
       <c r="B42" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="C42">
         <v>6076</v>
       </c>
     </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>41</v>
+      </c>
       <c r="B43" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="C43">
         <v>6157</v>
       </c>
     </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>42</v>
+      </c>
       <c r="B44" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="C44">
         <v>6208</v>
       </c>
     </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>43</v>
+      </c>
       <c r="B45" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="C45">
         <v>6154</v>
       </c>
     </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>44</v>
+      </c>
       <c r="B46" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="C46">
         <v>6211</v>
       </c>
     </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>45</v>
+      </c>
       <c r="B47" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="C47">
         <v>6056</v>
       </c>
     </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>46</v>
+      </c>
       <c r="B48" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="C48">
         <v>6055</v>
       </c>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>47</v>
+      </c>
       <c r="B49" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="C49">
         <v>6153</v>
       </c>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>48</v>
+      </c>
       <c r="B50" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="C50">
         <v>6069</v>
       </c>
     </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>49</v>
+      </c>
       <c r="B51" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="C51">
         <v>6112</v>
       </c>
     </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>50</v>
+      </c>
       <c r="B52" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="C52">
         <v>6149</v>
       </c>
     </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>51</v>
+      </c>
       <c r="B53" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="C53">
         <v>6028</v>
       </c>
     </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>52</v>
+      </c>
       <c r="B54" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="C54">
         <v>6100</v>
       </c>
     </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>53</v>
+      </c>
       <c r="B55" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="C55">
         <v>6036</v>
       </c>
     </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>54</v>
+      </c>
       <c r="B56" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="C56">
         <v>6122</v>
       </c>
     </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>55</v>
+      </c>
       <c r="B57" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="C57">
         <v>6167</v>
       </c>
     </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>56</v>
+      </c>
       <c r="B58" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="C58">
         <v>6111</v>
       </c>
     </row>
-    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>57</v>
+      </c>
       <c r="B59" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="C59">
         <v>6111</v>
       </c>
     </row>
-    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>58</v>
+      </c>
       <c r="B60" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="C60">
         <v>6155</v>
       </c>
     </row>
-    <row r="61" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>59</v>
+      </c>
       <c r="B61" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="C61">
         <v>6107</v>
       </c>
     </row>
-    <row r="62" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>60</v>
+      </c>
       <c r="B62" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="C62">
         <v>6033</v>
       </c>
     </row>
-    <row r="63" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>61</v>
+      </c>
       <c r="B63" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="C63">
         <v>6122</v>
       </c>
     </row>
-    <row r="64" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>62</v>
+      </c>
       <c r="B64" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="C64">
         <v>6020</v>
       </c>
     </row>
-    <row r="65" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>63</v>
+      </c>
       <c r="B65" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="C65">
         <v>6101</v>
       </c>
     </row>
-    <row r="66" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>64</v>
+      </c>
       <c r="B66" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="C66">
         <v>6076</v>
       </c>
     </row>
-    <row r="67" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>65</v>
+      </c>
       <c r="B67" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="C67">
         <v>6031</v>
       </c>
     </row>
-    <row r="68" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>66</v>
+      </c>
       <c r="B68" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="C68">
         <v>6167</v>
       </c>
     </row>
-    <row r="69" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>67</v>
+      </c>
       <c r="B69" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="C69">
         <v>6055</v>
       </c>
     </row>
-    <row r="70" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>68</v>
+      </c>
       <c r="B70" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="C70">
         <v>6111</v>
       </c>
     </row>
-    <row r="71" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>69</v>
+      </c>
       <c r="B71" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="C71">
         <v>6018</v>
       </c>
     </row>
-    <row r="72" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>70</v>
+      </c>
       <c r="B72" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
       <c r="C72">
         <v>6015</v>
       </c>
     </row>
-    <row r="73" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>71</v>
+      </c>
       <c r="B73" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="C73">
         <v>6010</v>
       </c>
     </row>
-    <row r="74" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>72</v>
+      </c>
       <c r="B74" t="s">
-        <v>349</v>
+        <v>341</v>
       </c>
       <c r="C74">
         <v>6030</v>
       </c>
     </row>
-    <row r="75" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>73</v>
+      </c>
       <c r="B75" t="s">
-        <v>350</v>
+        <v>342</v>
       </c>
       <c r="C75">
         <v>6105</v>
       </c>
     </row>
-    <row r="76" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>74</v>
+      </c>
       <c r="B76" t="s">
-        <v>352</v>
+        <v>344</v>
       </c>
       <c r="C76">
         <v>6152</v>
       </c>
     </row>
-    <row r="77" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>75</v>
+      </c>
       <c r="B77" t="s">
-        <v>351</v>
+        <v>343</v>
       </c>
       <c r="C77">
         <v>6027</v>
       </c>
     </row>
-    <row r="78" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>76</v>
+      </c>
       <c r="B78" t="s">
-        <v>353</v>
+        <v>345</v>
       </c>
       <c r="C78">
         <v>6210</v>
       </c>
     </row>
-    <row r="79" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>77</v>
+      </c>
       <c r="B79" t="s">
-        <v>354</v>
+        <v>346</v>
       </c>
       <c r="C79">
         <v>6166</v>
       </c>
     </row>
-    <row r="80" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>78</v>
+      </c>
       <c r="B80" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
       <c r="C80">
         <v>6163</v>
       </c>
     </row>
-    <row r="81" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>79</v>
+      </c>
       <c r="B81" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="C81">
         <v>6050</v>
       </c>
     </row>
-    <row r="82" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>80</v>
+      </c>
       <c r="B82" t="s">
-        <v>357</v>
+        <v>349</v>
       </c>
       <c r="C82">
         <v>6168</v>
       </c>
     </row>
-    <row r="83" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>81</v>
+      </c>
       <c r="B83" t="s">
-        <v>358</v>
+        <v>350</v>
       </c>
       <c r="C83">
         <v>6011</v>
       </c>
     </row>
-    <row r="84" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>82</v>
+      </c>
       <c r="B84" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="C84">
         <v>6025</v>
       </c>
     </row>
-    <row r="85" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>83</v>
+      </c>
       <c r="B85" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C85">
         <v>6009</v>
       </c>
     </row>
-    <row r="86" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>84</v>
+      </c>
       <c r="B86" t="s">
-        <v>379</v>
+        <v>371</v>
       </c>
       <c r="C86">
         <v>6067</v>
       </c>
     </row>
-    <row r="87" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>85</v>
+      </c>
       <c r="B87" t="s">
-        <v>378</v>
+        <v>370</v>
       </c>
       <c r="C87">
         <v>6028</v>
       </c>
     </row>
-    <row r="88" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>86</v>
+      </c>
       <c r="B88" t="s">
-        <v>377</v>
+        <v>369</v>
       </c>
       <c r="C88">
         <v>6008</v>
       </c>
     </row>
-    <row r="89" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>87</v>
+      </c>
       <c r="B89" t="s">
-        <v>376</v>
+        <v>368</v>
       </c>
       <c r="C89">
         <v>6009</v>
       </c>
     </row>
-    <row r="90" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>88</v>
+      </c>
       <c r="B90" t="s">
-        <v>375</v>
+        <v>367</v>
       </c>
       <c r="C90">
         <v>6065</v>
       </c>
     </row>
-    <row r="91" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>89</v>
+      </c>
       <c r="B91" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
       <c r="C91">
         <v>6122</v>
       </c>
     </row>
-    <row r="92" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>90</v>
+      </c>
       <c r="B92" t="s">
-        <v>373</v>
+        <v>365</v>
       </c>
       <c r="C92">
         <v>6070</v>
       </c>
     </row>
-    <row r="93" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>91</v>
+      </c>
       <c r="B93" t="s">
-        <v>372</v>
+        <v>364</v>
       </c>
       <c r="C93">
         <v>6211</v>
       </c>
     </row>
-    <row r="94" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>92</v>
+      </c>
       <c r="B94" t="s">
-        <v>371</v>
+        <v>363</v>
       </c>
       <c r="C94">
         <v>6055</v>
       </c>
     </row>
-    <row r="95" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>93</v>
+      </c>
       <c r="B95" t="s">
-        <v>370</v>
+        <v>362</v>
       </c>
       <c r="C95">
         <v>6059</v>
       </c>
     </row>
-    <row r="96" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>94</v>
+      </c>
       <c r="B96" t="s">
-        <v>369</v>
+        <v>361</v>
       </c>
       <c r="C96">
         <v>6018</v>
       </c>
     </row>
-    <row r="97" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>95</v>
+      </c>
       <c r="B97" t="s">
-        <v>368</v>
+        <v>360</v>
       </c>
       <c r="C97">
         <v>6210</v>
       </c>
     </row>
-    <row r="98" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>96</v>
+      </c>
       <c r="B98" t="s">
-        <v>367</v>
+        <v>359</v>
       </c>
       <c r="C98">
         <v>6023</v>
       </c>
     </row>
-    <row r="99" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>97</v>
+      </c>
       <c r="B99" t="s">
-        <v>366</v>
+        <v>358</v>
       </c>
       <c r="C99">
         <v>6107</v>
       </c>
     </row>
-    <row r="100" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>98</v>
+      </c>
       <c r="B100" t="s">
-        <v>365</v>
+        <v>357</v>
       </c>
       <c r="C100">
         <v>6158</v>
       </c>
     </row>
-    <row r="101" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>99</v>
+      </c>
       <c r="B101" t="s">
-        <v>364</v>
+        <v>356</v>
       </c>
       <c r="C101">
         <v>6004</v>
       </c>
     </row>
-    <row r="102" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>100</v>
+      </c>
       <c r="B102" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
       <c r="C102">
         <v>6168</v>
       </c>
     </row>
-    <row r="103" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>101</v>
+      </c>
       <c r="B103" t="s">
-        <v>362</v>
+        <v>354</v>
       </c>
       <c r="C103">
         <v>6101</v>
       </c>
     </row>
-    <row r="104" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>102</v>
+      </c>
       <c r="B104" t="s">
-        <v>361</v>
+        <v>353</v>
       </c>
       <c r="C104">
         <v>6054</v>
       </c>
     </row>
-    <row r="105" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>103</v>
+      </c>
       <c r="B105" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
       <c r="C105">
         <v>6027</v>
       </c>
     </row>
-    <row r="106" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>104</v>
+      </c>
       <c r="B106" t="s">
-        <v>359</v>
+        <v>351</v>
       </c>
       <c r="C106">
         <v>6034</v>
       </c>
     </row>
-    <row r="107" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>105</v>
+      </c>
       <c r="B107" t="s">
-        <v>346</v>
+        <v>338</v>
       </c>
       <c r="C107">
         <v>6069</v>
       </c>
     </row>
-    <row r="108" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>106</v>
+      </c>
       <c r="B108" t="s">
-        <v>345</v>
+        <v>337</v>
       </c>
       <c r="C108">
         <v>6062</v>
       </c>
     </row>
-    <row r="109" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109">
+        <v>107</v>
+      </c>
       <c r="B109" t="s">
-        <v>344</v>
+        <v>336</v>
       </c>
       <c r="C109">
         <v>6210</v>
       </c>
     </row>
-    <row r="110" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110">
+        <v>108</v>
+      </c>
       <c r="B110" t="s">
-        <v>343</v>
+        <v>335</v>
       </c>
       <c r="C110">
         <v>6208</v>
       </c>
     </row>
-    <row r="111" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <v>109</v>
+      </c>
       <c r="B111" t="s">
-        <v>342</v>
+        <v>334</v>
       </c>
       <c r="C111">
         <v>6210</v>
       </c>
     </row>
-    <row r="112" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112">
+        <v>110</v>
+      </c>
       <c r="B112" t="s">
-        <v>341</v>
+        <v>333</v>
       </c>
       <c r="C112">
         <v>6148</v>
       </c>
     </row>
-    <row r="113" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <v>111</v>
+      </c>
       <c r="B113" t="s">
-        <v>340</v>
+        <v>332</v>
       </c>
       <c r="C113">
         <v>6014</v>
       </c>
     </row>
-    <row r="114" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114">
+        <v>112</v>
+      </c>
       <c r="B114" t="s">
-        <v>339</v>
+        <v>331</v>
       </c>
       <c r="C114">
         <v>6112</v>
       </c>
     </row>
-    <row r="115" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115">
+        <v>113</v>
+      </c>
       <c r="B115" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
       <c r="C115">
         <v>6058</v>
       </c>
     </row>
-    <row r="116" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116">
+        <v>114</v>
+      </c>
       <c r="B116" t="s">
-        <v>337</v>
+        <v>329</v>
       </c>
       <c r="C116">
         <v>6160</v>
       </c>
     </row>
-    <row r="117" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117">
+        <v>115</v>
+      </c>
       <c r="B117" t="s">
-        <v>336</v>
+        <v>328</v>
       </c>
       <c r="C117">
         <v>6209</v>
       </c>
     </row>
-    <row r="118" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <v>116</v>
+      </c>
       <c r="B118" t="s">
-        <v>335</v>
+        <v>327</v>
       </c>
       <c r="C118">
         <v>6064</v>
       </c>
     </row>
-    <row r="119" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <v>117</v>
+      </c>
       <c r="B119" t="s">
-        <v>334</v>
+        <v>326</v>
       </c>
       <c r="C119">
         <v>6071</v>
       </c>
     </row>
-    <row r="120" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <v>118</v>
+      </c>
       <c r="B120" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
       <c r="C120">
         <v>6016</v>
       </c>
     </row>
-    <row r="121" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121">
+        <v>119</v>
+      </c>
       <c r="B121" t="s">
-        <v>332</v>
+        <v>324</v>
       </c>
       <c r="C121">
         <v>6077</v>
       </c>
     </row>
-    <row r="122" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122">
+        <v>120</v>
+      </c>
       <c r="B122" t="s">
-        <v>331</v>
+        <v>323</v>
       </c>
       <c r="C122">
         <v>6174</v>
       </c>
     </row>
-    <row r="123" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A123">
+        <v>121</v>
+      </c>
       <c r="B123" t="s">
-        <v>330</v>
+        <v>322</v>
       </c>
       <c r="C123">
         <v>6076</v>
       </c>
     </row>
-    <row r="124" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A124">
+        <v>122</v>
+      </c>
       <c r="B124" t="s">
-        <v>329</v>
+        <v>321</v>
       </c>
       <c r="C124">
         <v>6556</v>
       </c>
     </row>
-    <row r="125" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A125">
+        <v>123</v>
+      </c>
       <c r="B125" t="s">
-        <v>328</v>
+        <v>320</v>
       </c>
       <c r="C125">
         <v>6110</v>
       </c>
     </row>
-    <row r="126" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A126">
+        <v>124</v>
+      </c>
       <c r="B126" t="s">
-        <v>327</v>
+        <v>319</v>
       </c>
       <c r="C126">
         <v>6210</v>
       </c>
     </row>
-    <row r="127" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A127">
+        <v>125</v>
+      </c>
       <c r="B127" t="s">
-        <v>326</v>
+        <v>318</v>
       </c>
       <c r="C127">
         <v>6056</v>
       </c>
     </row>
-    <row r="128" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A128">
+        <v>126</v>
+      </c>
       <c r="B128" t="s">
-        <v>325</v>
+        <v>317</v>
       </c>
       <c r="C128">
         <v>6024</v>
       </c>
     </row>
-    <row r="129" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A129">
+        <v>127</v>
+      </c>
       <c r="B129" t="s">
-        <v>324</v>
+        <v>316</v>
       </c>
       <c r="C129">
         <v>6055</v>
       </c>
     </row>
-    <row r="130" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A130">
+        <v>128</v>
+      </c>
       <c r="B130" t="s">
-        <v>323</v>
+        <v>315</v>
       </c>
       <c r="C130">
         <v>6018</v>
       </c>
     </row>
-    <row r="131" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A131">
+        <v>129</v>
+      </c>
       <c r="B131" t="s">
-        <v>322</v>
+        <v>314</v>
       </c>
       <c r="C131">
         <v>6076</v>
       </c>
     </row>
-    <row r="132" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A132">
+        <v>130</v>
+      </c>
       <c r="B132" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
       <c r="C132">
         <v>6210</v>
       </c>
     </row>
-    <row r="133" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A133">
+        <v>131</v>
+      </c>
       <c r="B133" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="C133">
         <v>6022</v>
       </c>
     </row>
-    <row r="134" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A134">
+        <v>132</v>
+      </c>
       <c r="B134" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
       <c r="C134">
         <v>6163</v>
       </c>
     </row>
-    <row r="135" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A135">
+        <v>133</v>
+      </c>
       <c r="B135" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="C135">
         <v>6164</v>
       </c>
     </row>
-    <row r="136" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A136">
+        <v>134</v>
+      </c>
       <c r="B136" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="C136">
         <v>6112</v>
       </c>
     </row>
-    <row r="137" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A137">
+        <v>135</v>
+      </c>
       <c r="B137" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="C137">
         <v>6112</v>
       </c>
     </row>
-    <row r="138" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A138">
+        <v>136</v>
+      </c>
       <c r="B138" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="C138">
         <v>6055</v>
       </c>
     </row>
-    <row r="139" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A139">
+        <v>137</v>
+      </c>
       <c r="B139" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
       <c r="C139">
         <v>6027</v>
       </c>
     </row>
-    <row r="140" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A140">
+        <v>138</v>
+      </c>
       <c r="B140" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
       <c r="C140">
         <v>6056</v>
       </c>
     </row>
-    <row r="141" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A141">
+        <v>139</v>
+      </c>
       <c r="B141" t="s">
-        <v>312</v>
+        <v>304</v>
       </c>
       <c r="C141">
         <v>6166</v>
       </c>
     </row>
-    <row r="142" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A142">
+        <v>140</v>
+      </c>
       <c r="B142" t="s">
-        <v>311</v>
+        <v>303</v>
       </c>
       <c r="C142">
         <v>6055</v>
       </c>
     </row>
-    <row r="143" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A143">
+        <v>141</v>
+      </c>
       <c r="B143" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="C143">
         <v>6017</v>
       </c>
     </row>
-    <row r="144" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A144">
+        <v>142</v>
+      </c>
       <c r="B144" t="s">
-        <v>309</v>
+        <v>301</v>
       </c>
       <c r="C144">
         <v>6056</v>
       </c>
     </row>
-    <row r="145" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A145">
+        <v>143</v>
+      </c>
       <c r="B145" t="s">
-        <v>308</v>
+        <v>300</v>
       </c>
       <c r="C145">
         <v>6057</v>
       </c>
     </row>
-    <row r="146" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A146">
+        <v>144</v>
+      </c>
       <c r="B146" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
       <c r="C146">
         <v>6003</v>
       </c>
     </row>
-    <row r="147" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A147">
+        <v>145</v>
+      </c>
       <c r="B147" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="C147">
         <v>6112</v>
       </c>
     </row>
-    <row r="148" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A148">
+        <v>146</v>
+      </c>
       <c r="B148" t="s">
-        <v>305</v>
+        <v>297</v>
       </c>
       <c r="C148">
         <v>6025</v>
       </c>
     </row>
-    <row r="149" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A149">
+        <v>147</v>
+      </c>
       <c r="B149" t="s">
-        <v>304</v>
+        <v>296</v>
       </c>
       <c r="C149">
         <v>6168</v>
       </c>
     </row>
-    <row r="150" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A150">
+        <v>148</v>
+      </c>
       <c r="B150" t="s">
-        <v>303</v>
+        <v>295</v>
       </c>
       <c r="C150">
         <v>6163</v>
       </c>
     </row>
-    <row r="151" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A151">
+        <v>149</v>
+      </c>
       <c r="B151" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="C151">
         <v>6065</v>
       </c>
     </row>
-    <row r="152" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A152">
+        <v>150</v>
+      </c>
       <c r="B152" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="C152">
         <v>6165</v>
       </c>
     </row>
-    <row r="153" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A153">
+        <v>151</v>
+      </c>
       <c r="B153" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="C153">
         <v>6125</v>
       </c>
     </row>
-    <row r="154" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A154">
+        <v>152</v>
+      </c>
       <c r="B154" t="s">
-        <v>299</v>
+        <v>291</v>
       </c>
       <c r="C154">
         <v>6071</v>
       </c>
     </row>
-    <row r="155" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A155">
+        <v>153</v>
+      </c>
       <c r="B155" t="s">
-        <v>298</v>
+        <v>290</v>
       </c>
       <c r="C155">
         <v>6110</v>
       </c>
     </row>
-    <row r="156" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A156">
+        <v>154</v>
+      </c>
       <c r="B156" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
       <c r="C156">
         <v>6028</v>
       </c>
     </row>
-    <row r="157" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A157">
+        <v>155</v>
+      </c>
       <c r="B157" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="C157">
         <v>6052</v>
       </c>
     </row>
-    <row r="158" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A158">
+        <v>156</v>
+      </c>
       <c r="B158" s="1" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="C158">
         <v>6018</v>
       </c>
     </row>
-    <row r="159" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A159">
+        <v>157</v>
+      </c>
       <c r="B159" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="C159">
         <v>6077</v>
       </c>
     </row>
-    <row r="160" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A160">
+        <v>158</v>
+      </c>
       <c r="B160" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="C160">
         <v>6164</v>
       </c>
     </row>
-    <row r="161" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A161">
+        <v>159</v>
+      </c>
       <c r="B161" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
       <c r="C161">
         <v>6056</v>
       </c>
     </row>
-    <row r="162" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A162">
+        <v>160</v>
+      </c>
       <c r="B162" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
       <c r="C162">
         <v>6036</v>
       </c>
     </row>
-    <row r="163" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A163">
+        <v>161</v>
+      </c>
       <c r="B163" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="C163">
         <v>6014</v>
       </c>
     </row>
-    <row r="164" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A164">
+        <v>162</v>
+      </c>
       <c r="B164" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="C164">
         <v>6027</v>
       </c>
     </row>
-    <row r="165" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A165">
+        <v>163</v>
+      </c>
       <c r="B165" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="C165">
         <v>6060</v>
       </c>
     </row>
-    <row r="166" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A166">
+        <v>164</v>
+      </c>
       <c r="B166" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
       <c r="C166">
         <v>6076</v>
       </c>
     </row>
-    <row r="167" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A167">
+        <v>165</v>
+      </c>
       <c r="B167" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="C167">
         <v>6025</v>
       </c>
     </row>
-    <row r="168" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A168">
+        <v>166</v>
+      </c>
       <c r="B168" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="C168">
         <v>6152</v>
       </c>
     </row>
-    <row r="169" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A169">
+        <v>167</v>
+      </c>
       <c r="B169" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="C169">
         <v>6163</v>
       </c>
     </row>
-    <row r="170" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A170">
+        <v>168</v>
+      </c>
       <c r="B170" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="C170">
         <v>6176</v>
       </c>
     </row>
-    <row r="171" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A171">
+        <v>169</v>
+      </c>
       <c r="B171" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="C171">
         <v>6111</v>
       </c>
     </row>
-    <row r="172" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A172">
+        <v>170</v>
+      </c>
       <c r="B172" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
       <c r="C172">
         <v>6010</v>
       </c>
     </row>
-    <row r="173" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A173">
+        <v>171</v>
+      </c>
       <c r="B173" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="C173">
         <v>6122</v>
       </c>
     </row>
-    <row r="174" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A174">
+        <v>172</v>
+      </c>
       <c r="B174" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="C174">
         <v>6018</v>
       </c>
     </row>
-    <row r="175" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A175">
+        <v>173</v>
+      </c>
       <c r="B175" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="C175">
         <v>6111</v>
       </c>
     </row>
-    <row r="176" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A176">
+        <v>174</v>
+      </c>
       <c r="B176" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="C176">
         <v>6151</v>
       </c>
     </row>
-    <row r="177" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A177">
+        <v>175</v>
+      </c>
       <c r="B177" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="C177">
         <v>6107</v>
       </c>
     </row>
-    <row r="178" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A178">
+        <v>176</v>
+      </c>
       <c r="B178" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="C178">
         <v>6105</v>
       </c>
     </row>
-    <row r="179" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A179">
+        <v>177</v>
+      </c>
       <c r="B179" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="C179">
         <v>6054</v>
       </c>
     </row>
-    <row r="180" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A180">
+        <v>178</v>
+      </c>
       <c r="B180" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="C180">
         <v>6005</v>
       </c>
     </row>
-    <row r="181" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A181">
+        <v>179</v>
+      </c>
       <c r="B181" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="C181">
         <v>6026</v>
       </c>
     </row>
-    <row r="182" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A182">
+        <v>180</v>
+      </c>
       <c r="B182" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="C182">
         <v>6028</v>
       </c>
     </row>
-    <row r="183" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A183">
+        <v>181</v>
+      </c>
       <c r="B183" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="C183">
         <v>6064</v>
       </c>
     </row>
-    <row r="184" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A184">
+        <v>182</v>
+      </c>
       <c r="B184" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="C184">
         <v>6056</v>
       </c>
     </row>
-    <row r="185" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A185">
+        <v>183</v>
+      </c>
       <c r="B185" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="C185">
         <v>6167</v>
       </c>
     </row>
-    <row r="186" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A186">
+        <v>184</v>
+      </c>
       <c r="B186" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="C186">
         <v>6167</v>
       </c>
     </row>
-    <row r="187" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A187">
+        <v>185</v>
+      </c>
       <c r="B187" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="C187">
         <v>6167</v>
       </c>
     </row>
-    <row r="188" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A188">
+        <v>186</v>
+      </c>
       <c r="B188" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="C188">
         <v>6180</v>
       </c>
     </row>
-    <row r="189" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A189">
+        <v>187</v>
+      </c>
       <c r="B189" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="C189">
         <v>6065</v>
       </c>
     </row>
-    <row r="190" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A190">
+        <v>188</v>
+      </c>
       <c r="B190" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="C190">
         <v>6147</v>
       </c>
     </row>
-    <row r="191" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A191">
+        <v>189</v>
+      </c>
       <c r="B191" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="C191">
         <v>6100</v>
       </c>
     </row>
-    <row r="192" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A192">
+        <v>190</v>
+      </c>
       <c r="B192" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="C192">
         <v>6170</v>
       </c>
     </row>
-    <row r="193" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A193">
+        <v>191</v>
+      </c>
       <c r="B193" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="C193">
         <v>6007</v>
       </c>
     </row>
-    <row r="194" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A194">
+        <v>192</v>
+      </c>
       <c r="B194" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="C194">
         <v>6149</v>
       </c>
     </row>
-    <row r="195" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A195">
+        <v>193</v>
+      </c>
       <c r="B195" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="C195">
         <v>6076</v>
       </c>
     </row>
-    <row r="196" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A196">
+        <v>194</v>
+      </c>
       <c r="B196" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="C196">
         <v>6079</v>
       </c>
     </row>
-    <row r="197" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A197">
+        <v>195</v>
+      </c>
       <c r="B197" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="C197">
         <v>6054</v>
       </c>
     </row>
-    <row r="198" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A198">
+        <v>196</v>
+      </c>
       <c r="B198" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="C198">
         <v>6147</v>
       </c>
     </row>
-    <row r="199" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A199">
+        <v>197</v>
+      </c>
       <c r="B199" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="C199">
         <v>6109</v>
       </c>
     </row>
-    <row r="200" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A200">
+        <v>198</v>
+      </c>
       <c r="B200" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="C200">
         <v>6065</v>
       </c>
     </row>
-    <row r="201" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A201">
+        <v>199</v>
+      </c>
       <c r="B201" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="C201">
         <v>6210</v>
       </c>
     </row>
-    <row r="202" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A202">
+        <v>200</v>
+      </c>
       <c r="B202" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="C202">
         <v>6072</v>
       </c>
     </row>
-    <row r="203" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A203">
+        <v>201</v>
+      </c>
       <c r="B203" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="C203">
         <v>6057</v>
       </c>
     </row>
-    <row r="204" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A204">
+        <v>202</v>
+      </c>
       <c r="B204" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="C204">
         <v>6090</v>
       </c>
     </row>
-    <row r="205" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A205">
+        <v>203</v>
+      </c>
       <c r="B205" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="C205">
         <v>6167</v>
       </c>
     </row>
-    <row r="206" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A206">
+        <v>204</v>
+      </c>
       <c r="B206" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="C206">
         <v>6210</v>
       </c>
     </row>
-    <row r="207" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A207">
+        <v>205</v>
+      </c>
       <c r="B207" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="C207">
         <v>6152</v>
       </c>
     </row>
-    <row r="208" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A208">
+        <v>206</v>
+      </c>
       <c r="B208" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="C208">
         <v>6064</v>
       </c>
     </row>
-    <row r="209" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A209">
+        <v>207</v>
+      </c>
       <c r="B209" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="C209">
         <v>6125</v>
       </c>
     </row>
-    <row r="210" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A210">
+        <v>208</v>
+      </c>
       <c r="B210" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="C210">
         <v>6078</v>
       </c>
     </row>
-    <row r="211" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A211">
+        <v>209</v>
+      </c>
       <c r="B211" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="C211">
         <v>6020</v>
       </c>
     </row>
-    <row r="212" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A212">
+        <v>210</v>
+      </c>
       <c r="B212" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="C212">
         <v>6110</v>
       </c>
     </row>
-    <row r="213" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A213">
+        <v>211</v>
+      </c>
       <c r="B213" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="C213">
         <v>6051</v>
       </c>
     </row>
-    <row r="214" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A214">
+        <v>212</v>
+      </c>
       <c r="B214" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="C214">
         <v>6210</v>
       </c>
     </row>
-    <row r="215" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A215">
+        <v>213</v>
+      </c>
       <c r="B215" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="C215">
         <v>6167</v>
       </c>
     </row>
-    <row r="216" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A216">
+        <v>214</v>
+      </c>
       <c r="B216" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="C216">
         <v>6079</v>
       </c>
     </row>
-    <row r="217" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A217">
+        <v>215</v>
+      </c>
       <c r="B217" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="C217">
         <v>6156</v>
       </c>
     </row>
-    <row r="218" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A218">
+        <v>216</v>
+      </c>
       <c r="B218" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="C218">
         <v>6050</v>
       </c>
     </row>
-    <row r="219" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A219">
+        <v>217</v>
+      </c>
       <c r="B219" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="C219">
         <v>6030</v>
       </c>
     </row>
-    <row r="220" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A220">
+        <v>218</v>
+      </c>
       <c r="B220" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="C220">
         <v>6056</v>
       </c>
     </row>
-    <row r="221" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A221">
+        <v>219</v>
+      </c>
       <c r="B221" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="C221">
         <v>6056</v>
       </c>
     </row>
-    <row r="222" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A222">
+        <v>220</v>
+      </c>
       <c r="B222" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="C222">
         <v>6056</v>
       </c>
     </row>
-    <row r="223" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A223">
+        <v>221</v>
+      </c>
       <c r="B223" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="C223">
         <v>6056</v>
       </c>
     </row>
-    <row r="224" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A224">
+        <v>222</v>
+      </c>
       <c r="B224" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="C224">
         <v>6030</v>
       </c>
     </row>
-    <row r="225" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A225">
+        <v>223</v>
+      </c>
       <c r="B225" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="C225">
         <v>6061</v>
       </c>
     </row>
-    <row r="226" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A226">
+        <v>224</v>
+      </c>
       <c r="B226" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="C226">
         <v>6062</v>
       </c>
     </row>
-    <row r="227" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A227">
+        <v>225</v>
+      </c>
       <c r="B227" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="C227">
         <v>6012</v>
       </c>
     </row>
-    <row r="228" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A228">
+        <v>226</v>
+      </c>
       <c r="B228" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="C228">
         <v>6010</v>
       </c>
     </row>
-    <row r="229" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A229">
+        <v>227</v>
+      </c>
       <c r="B229" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="C229">
         <v>6016</v>
       </c>
     </row>
-    <row r="230" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A230">
+        <v>228</v>
+      </c>
       <c r="B230" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="C230">
         <v>6082</v>
       </c>
     </row>
-    <row r="231" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A231">
+        <v>229</v>
+      </c>
       <c r="B231" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="C231">
         <v>6050</v>
       </c>
     </row>
-    <row r="232" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A232">
+        <v>230</v>
+      </c>
       <c r="B232" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="C232">
         <v>6112</v>
       </c>
     </row>
-    <row r="233" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A233">
+        <v>231</v>
+      </c>
       <c r="B233" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="C233">
         <v>6153</v>
       </c>
     </row>
-    <row r="234" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A234">
+        <v>232</v>
+      </c>
       <c r="B234" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="C234">
         <v>6112</v>
       </c>
     </row>
-    <row r="235" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A235">
+        <v>233</v>
+      </c>
       <c r="B235" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="C235">
         <v>6027</v>
       </c>
     </row>
-    <row r="236" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A236">
+        <v>234</v>
+      </c>
       <c r="B236" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="C236">
         <v>6073</v>
       </c>
     </row>
-    <row r="237" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A237">
+        <v>235</v>
+      </c>
       <c r="B237" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="C237">
         <v>6166</v>
       </c>
     </row>
-    <row r="238" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A238">
+        <v>236</v>
+      </c>
       <c r="B238" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="C238">
         <v>6150</v>
       </c>
     </row>
-    <row r="239" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A239">
+        <v>237</v>
+      </c>
       <c r="B239" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="C239">
         <v>6154</v>
       </c>
     </row>
-    <row r="240" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A240">
+        <v>238</v>
+      </c>
       <c r="B240" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="C240">
         <v>6165</v>
       </c>
     </row>
-    <row r="241" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A241">
+        <v>239</v>
+      </c>
       <c r="B241" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="C241">
         <v>6009</v>
       </c>
     </row>
-    <row r="242" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A242">
+        <v>240</v>
+      </c>
       <c r="B242" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="C242">
         <v>6031</v>
       </c>
     </row>
-    <row r="243" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A243">
+        <v>241</v>
+      </c>
       <c r="B243" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="C243">
         <v>6208</v>
       </c>
     </row>
-    <row r="244" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A244">
+        <v>242</v>
+      </c>
       <c r="B244" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="C244">
         <v>6061</v>
       </c>
     </row>
-    <row r="245" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A245">
+        <v>243</v>
+      </c>
       <c r="B245" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="C245">
         <v>6062</v>
       </c>
     </row>
-    <row r="246" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A246">
+        <v>244</v>
+      </c>
       <c r="B246" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="C246">
         <v>6020</v>
       </c>
     </row>
-    <row r="247" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A247">
+        <v>245</v>
+      </c>
       <c r="B247" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="C247">
         <v>6163</v>
       </c>
     </row>
-    <row r="248" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A248">
+        <v>246</v>
+      </c>
       <c r="B248" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="C248">
         <v>6159</v>
       </c>
     </row>
-    <row r="249" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A249">
+        <v>247</v>
+      </c>
       <c r="B249" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="C249">
         <v>6163</v>
       </c>
     </row>
-    <row r="250" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A250">
+        <v>248</v>
+      </c>
       <c r="B250" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="C250">
         <v>6006</v>
       </c>
     </row>
-    <row r="251" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A251">
+        <v>249</v>
+      </c>
       <c r="B251" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="C251">
         <v>6208</v>
       </c>
     </row>
-    <row r="252" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A252">
+        <v>250</v>
+      </c>
       <c r="B252" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="C252">
         <v>6003</v>
       </c>
     </row>
-    <row r="253" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A253">
+        <v>251</v>
+      </c>
       <c r="B253" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="C253">
         <v>6032</v>
       </c>
     </row>
-    <row r="254" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A254">
+        <v>252</v>
+      </c>
       <c r="B254" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="C254">
         <v>6163</v>
       </c>
     </row>
-    <row r="255" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A255">
+        <v>253</v>
+      </c>
       <c r="B255" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="C255">
         <v>6121</v>
       </c>
     </row>
-    <row r="256" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A256">
+        <v>254</v>
+      </c>
       <c r="B256" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="C256">
         <v>6208</v>
       </c>
     </row>
-    <row r="257" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A257">
+        <v>255</v>
+      </c>
       <c r="B257" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="C257">
         <v>6027</v>
       </c>
     </row>
-    <row r="258" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A258">
+        <v>256</v>
+      </c>
       <c r="B258" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="C258">
         <v>6121</v>
       </c>
     </row>
-    <row r="259" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A259">
+        <v>257</v>
+      </c>
       <c r="B259" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="C259">
         <v>6109</v>
       </c>
     </row>
-    <row r="260" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A260">
+        <v>258</v>
+      </c>
       <c r="B260" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="C260">
         <v>6167</v>
       </c>
     </row>
-    <row r="261" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A261">
+        <v>259</v>
+      </c>
       <c r="B261" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="C261">
         <v>6017</v>
       </c>
     </row>
-    <row r="262" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A262">
+        <v>260</v>
+      </c>
       <c r="B262" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="C262">
         <v>6025</v>
       </c>
     </row>
-    <row r="263" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A263">
+        <v>261</v>
+      </c>
       <c r="B263" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C263">
         <v>6157</v>
       </c>
     </row>
-    <row r="264" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A264">
+        <v>262</v>
+      </c>
       <c r="B264" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="C264">
         <v>6081</v>
       </c>
     </row>
-    <row r="265" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A265">
+        <v>263</v>
+      </c>
       <c r="B265" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="C265">
         <v>6180</v>
       </c>
     </row>
-    <row r="266" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A266">
+        <v>264</v>
+      </c>
       <c r="B266" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="C266">
         <v>6147</v>
       </c>
     </row>
-    <row r="267" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A267">
+        <v>265</v>
+      </c>
       <c r="B267" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="C267">
         <v>6167</v>
       </c>
     </row>
-    <row r="268" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A268">
+        <v>266</v>
+      </c>
       <c r="B268" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="C268">
         <v>6076</v>
       </c>
     </row>
-    <row r="269" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A269">
+        <v>267</v>
+      </c>
       <c r="B269" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="C269">
         <v>6065</v>
       </c>
     </row>
-    <row r="270" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A270">
+        <v>268</v>
+      </c>
       <c r="B270" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C270">
         <v>6011</v>
       </c>
     </row>
-    <row r="271" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A271">
+        <v>269</v>
+      </c>
       <c r="B271" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="C271">
         <v>6168</v>
       </c>
     </row>
-    <row r="272" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A272">
+        <v>270</v>
+      </c>
       <c r="B272" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="C272">
         <v>6000</v>
       </c>
     </row>
-    <row r="273" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A273">
+        <v>271</v>
+      </c>
       <c r="B273" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="C273">
         <v>6105</v>
       </c>
     </row>
-    <row r="274" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A274">
+        <v>272</v>
+      </c>
       <c r="B274" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="C274">
         <v>6112</v>
       </c>
     </row>
-    <row r="275" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A275">
+        <v>273</v>
+      </c>
       <c r="B275" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="C275">
         <v>6076</v>
       </c>
     </row>
-    <row r="276" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A276">
+        <v>274</v>
+      </c>
       <c r="B276" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="C276">
         <v>6076</v>
       </c>
     </row>
-    <row r="277" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A277">
+        <v>275</v>
+      </c>
       <c r="B277" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="C277">
         <v>6208</v>
       </c>
     </row>
-    <row r="278" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A278">
+        <v>276</v>
+      </c>
       <c r="B278" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="C278">
         <v>6163</v>
       </c>
     </row>
-    <row r="279" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A279">
+        <v>277</v>
+      </c>
       <c r="B279" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="C279">
         <v>6172</v>
       </c>
     </row>
-    <row r="280" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A280">
+        <v>278</v>
+      </c>
       <c r="B280" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="C280">
         <v>6167</v>
       </c>
     </row>
-    <row r="281" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A281">
+        <v>279</v>
+      </c>
       <c r="B281" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="C281">
         <v>6107</v>
       </c>
     </row>
-    <row r="282" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A282">
+        <v>280</v>
+      </c>
       <c r="B282" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="C282">
         <v>6030</v>
       </c>
     </row>
-    <row r="283" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A283">
+        <v>281</v>
+      </c>
       <c r="B283" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="C283">
         <v>6208</v>
       </c>
     </row>
-    <row r="284" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A284">
+        <v>282</v>
+      </c>
       <c r="B284" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="C284">
         <v>6056</v>
       </c>
     </row>
-    <row r="285" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A285">
+        <v>283</v>
+      </c>
       <c r="B285" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="C285">
         <v>6104</v>
       </c>
     </row>
-    <row r="286" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A286">
+        <v>284</v>
+      </c>
       <c r="B286" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="C286">
         <v>6076</v>
       </c>
     </row>
-    <row r="287" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A287">
+        <v>285</v>
+      </c>
       <c r="B287" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="C287">
         <v>6030</v>
       </c>
     </row>
-    <row r="288" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A288">
+        <v>286</v>
+      </c>
       <c r="B288" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="C288">
         <v>6148</v>
       </c>
     </row>
-    <row r="289" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A289">
+        <v>287</v>
+      </c>
       <c r="B289" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="C289">
         <v>6103</v>
       </c>
     </row>
-    <row r="290" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A290">
+        <v>288</v>
+      </c>
       <c r="B290" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="C290">
         <v>6168</v>
       </c>
     </row>
-    <row r="291" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A291">
+        <v>289</v>
+      </c>
       <c r="B291" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="C291">
         <v>6111</v>
       </c>
     </row>
-    <row r="292" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A292">
+        <v>290</v>
+      </c>
       <c r="B292" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="C292">
         <v>6148</v>
       </c>
     </row>
-    <row r="293" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A293">
+        <v>291</v>
+      </c>
       <c r="B293" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="C293">
         <v>6169</v>
       </c>
     </row>
-    <row r="294" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A294">
+        <v>292</v>
+      </c>
       <c r="B294" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="C294">
         <v>6102</v>
       </c>
     </row>
-    <row r="295" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A295">
+        <v>293</v>
+      </c>
       <c r="B295" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="C295">
         <v>6152</v>
       </c>
     </row>
-    <row r="296" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A296">
+        <v>294</v>
+      </c>
       <c r="B296" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="C296">
         <v>6163</v>
       </c>
     </row>
-    <row r="297" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A297">
+        <v>295</v>
+      </c>
       <c r="B297" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="C297">
         <v>6210</v>
       </c>
     </row>
-    <row r="298" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A298">
+        <v>296</v>
+      </c>
       <c r="B298" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="C298">
         <v>6074</v>
       </c>
     </row>
-    <row r="299" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A299">
+        <v>297</v>
+      </c>
       <c r="B299" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="C299">
         <v>6019</v>
       </c>
     </row>
-    <row r="300" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A300">
+        <v>298</v>
+      </c>
       <c r="B300" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="C300">
         <v>6173</v>
       </c>
     </row>
-    <row r="301" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A301">
+        <v>299</v>
+      </c>
       <c r="B301" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="C301">
         <v>6112</v>
       </c>
     </row>
-    <row r="302" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A302">
+        <v>300</v>
+      </c>
       <c r="B302" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="C302">
         <v>6148</v>
       </c>
     </row>
-    <row r="303" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A303">
+        <v>301</v>
+      </c>
       <c r="B303" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="C303">
         <v>6008</v>
       </c>
     </row>
-    <row r="304" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A304">
+        <v>302</v>
+      </c>
       <c r="B304" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="C304">
         <v>6169</v>
       </c>
     </row>
-    <row r="305" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A305">
+        <v>303</v>
+      </c>
       <c r="B305" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="C305">
         <v>6210</v>
       </c>
     </row>
-    <row r="306" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A306">
+        <v>304</v>
+      </c>
       <c r="B306" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="C306">
         <v>6065</v>
       </c>
     </row>
-    <row r="307" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A307">
+        <v>305</v>
+      </c>
       <c r="B307" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="C307">
         <v>6175</v>
       </c>
     </row>
-    <row r="308" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A308">
+        <v>306</v>
+      </c>
       <c r="B308" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="C308">
         <v>6020</v>
       </c>
     </row>
-    <row r="309" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A309">
+        <v>307</v>
+      </c>
       <c r="B309" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="C309">
         <v>6162</v>
       </c>
     </row>
-    <row r="310" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A310">
+        <v>308</v>
+      </c>
       <c r="B310" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="C310">
         <v>6055</v>
       </c>
     </row>
-    <row r="311" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A311">
+        <v>309</v>
+      </c>
       <c r="B311" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="C311">
         <v>6164</v>
       </c>
     </row>
-    <row r="312" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A312">
+        <v>310</v>
+      </c>
       <c r="B312" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="C312">
         <v>6151</v>
       </c>
     </row>
-    <row r="313" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A313">
+        <v>311</v>
+      </c>
       <c r="B313" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="C313">
         <v>6208</v>
       </c>
     </row>
-    <row r="314" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A314">
+        <v>312</v>
+      </c>
       <c r="B314" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="C314">
         <v>6110</v>
       </c>
     </row>
-    <row r="315" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A315">
+        <v>313</v>
+      </c>
       <c r="B315" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="C315">
         <v>6163</v>
       </c>
     </row>
-    <row r="316" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A316">
+        <v>314</v>
+      </c>
       <c r="B316" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C316">
         <v>6181</v>
       </c>
     </row>
-    <row r="317" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A317">
+        <v>315</v>
+      </c>
       <c r="B317" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="C317">
         <v>6021</v>
       </c>
     </row>
-    <row r="318" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A318">
+        <v>316</v>
+      </c>
       <c r="B318" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="C318">
         <v>6081</v>
       </c>
     </row>
-    <row r="319" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A319">
+        <v>317</v>
+      </c>
       <c r="B319" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="C319">
         <v>6056</v>
       </c>
     </row>
-    <row r="320" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A320">
+        <v>318</v>
+      </c>
       <c r="B320" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="C320">
         <v>6008</v>
       </c>
     </row>
-    <row r="321" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A321">
+        <v>319</v>
+      </c>
       <c r="B321" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="C321">
         <v>6164</v>
       </c>
     </row>
-    <row r="322" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A322">
+        <v>320</v>
+      </c>
       <c r="B322" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="C322">
         <v>6056</v>
       </c>
     </row>
-    <row r="323" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A323">
+        <v>321</v>
+      </c>
       <c r="B323" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="C323">
         <v>6010</v>
       </c>
     </row>
-    <row r="324" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A324">
+        <v>322</v>
+      </c>
       <c r="B324" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="C324">
         <v>6030</v>
       </c>
     </row>
-    <row r="325" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A325">
+        <v>323</v>
+      </c>
       <c r="B325" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="C325">
         <v>6065</v>
       </c>
     </row>
-    <row r="326" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A326">
+        <v>324</v>
+      </c>
       <c r="B326" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="C326">
         <v>6556</v>
       </c>
     </row>
-    <row r="327" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A327">
+        <v>325</v>
+      </c>
       <c r="B327" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="C327">
         <v>6167</v>
       </c>
     </row>
-    <row r="328" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A328">
+        <v>326</v>
+      </c>
       <c r="B328" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="C328">
         <v>6069</v>
       </c>
     </row>
-    <row r="329" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A329">
+        <v>327</v>
+      </c>
       <c r="B329" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="C329">
         <v>6108</v>
       </c>
     </row>
-    <row r="330" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A330">
+        <v>328</v>
+      </c>
       <c r="B330" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="C330">
         <v>6029</v>
       </c>
     </row>
-    <row r="331" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A331">
+        <v>329</v>
+      </c>
       <c r="B331" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="C331">
         <v>6060</v>
       </c>
     </row>
-    <row r="332" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A332">
+        <v>330</v>
+      </c>
       <c r="B332" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="C332">
         <v>6037</v>
       </c>
     </row>
-    <row r="333" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A333">
+        <v>331</v>
+      </c>
       <c r="B333" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="C333">
         <v>6069</v>
       </c>
     </row>
-    <row r="334" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A334">
+        <v>332</v>
+      </c>
       <c r="B334" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="C334">
         <v>6100</v>
       </c>
     </row>
-    <row r="335" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A335">
+        <v>333</v>
+      </c>
       <c r="B335" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="C335">
         <v>6056</v>
       </c>
     </row>
-    <row r="336" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A336">
+        <v>334</v>
+      </c>
       <c r="B336" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="C336">
         <v>6169</v>
       </c>
     </row>
-    <row r="337" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A337">
+        <v>335</v>
+      </c>
       <c r="B337" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="C337">
         <v>6076</v>
       </c>
     </row>
-    <row r="338" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A338">
+        <v>336</v>
+      </c>
       <c r="B338" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="C338">
         <v>6167</v>
       </c>
     </row>
-    <row r="339" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A339">
+        <v>337</v>
+      </c>
       <c r="B339" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="C339">
         <v>6065</v>
       </c>
     </row>
-    <row r="340" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A340">
+        <v>338</v>
+      </c>
       <c r="B340" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="C340">
         <v>6210</v>
       </c>
     </row>
-    <row r="341" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A341">
+        <v>339</v>
+      </c>
       <c r="B341" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="C341">
         <v>6065</v>
       </c>
     </row>
-    <row r="342" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A342">
+        <v>340</v>
+      </c>
       <c r="B342" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="C342">
         <v>6169</v>
       </c>
     </row>
-    <row r="343" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A343">
+        <v>341</v>
+      </c>
       <c r="B343" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C343">
         <v>6024</v>
       </c>
     </row>
-    <row r="344" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A344">
+        <v>342</v>
+      </c>
       <c r="B344" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="C344">
         <v>6152</v>
       </c>
     </row>
-    <row r="345" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A345">
+        <v>343</v>
+      </c>
       <c r="B345" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="C345">
         <v>6020</v>
       </c>
     </row>
-    <row r="346" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A346">
+        <v>344</v>
+      </c>
       <c r="B346" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="C346">
         <v>6107</v>
       </c>
     </row>
-    <row r="347" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A347">
+        <v>345</v>
+      </c>
       <c r="B347" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="C347">
         <v>6166</v>
       </c>
     </row>
-    <row r="348" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A348">
+        <v>346</v>
+      </c>
       <c r="B348" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="C348">
         <v>6170</v>
       </c>
     </row>
-    <row r="349" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A349">
+        <v>347</v>
+      </c>
       <c r="B349" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C349">
         <v>6106</v>
       </c>
     </row>
-    <row r="350" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A350">
+        <v>348</v>
+      </c>
       <c r="B350" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="C350">
         <v>6014</v>
       </c>
     </row>
-    <row r="351" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A351">
+        <v>349</v>
+      </c>
       <c r="B351" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="C351">
         <v>6019</v>
       </c>
     </row>
-    <row r="352" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A352">
+        <v>350</v>
+      </c>
       <c r="B352" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="C352">
         <v>6007</v>
       </c>
     </row>
-    <row r="353" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A353">
+        <v>351</v>
+      </c>
       <c r="B353" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="C353">
         <v>6005</v>
       </c>
     </row>
-    <row r="354" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A354">
+        <v>352</v>
+      </c>
       <c r="B354" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="C354">
         <v>6055</v>
       </c>
     </row>
-    <row r="355" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A355">
+        <v>353</v>
+      </c>
       <c r="B355" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="C355">
         <v>6111</v>
       </c>
     </row>
-    <row r="356" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A356">
+        <v>354</v>
+      </c>
       <c r="B356" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="C356">
         <v>6061</v>
       </c>
     </row>
-    <row r="357" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A357">
+        <v>355</v>
+      </c>
       <c r="B357" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C357">
         <v>6123</v>
       </c>
     </row>
-    <row r="358" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A358">
+        <v>356</v>
+      </c>
       <c r="B358" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="C358">
         <v>6162</v>
       </c>
     </row>
-    <row r="359" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A359">
+        <v>357</v>
+      </c>
       <c r="B359" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C359">
         <v>6068</v>
       </c>
     </row>
-    <row r="360" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A360">
+        <v>358</v>
+      </c>
       <c r="B360" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="C360">
         <v>6041</v>
       </c>
     </row>
-    <row r="361" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A361">
+        <v>359</v>
+      </c>
       <c r="B361" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="C361">
         <v>6156</v>
       </c>
     </row>
-    <row r="362" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A362">
+        <v>360</v>
+      </c>
       <c r="B362" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C362">
         <v>6155</v>
       </c>
     </row>
-    <row r="363" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A363">
+        <v>361</v>
+      </c>
       <c r="B363" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="C363">
         <v>6107</v>
       </c>
     </row>
-    <row r="364" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A364">
+        <v>362</v>
+      </c>
       <c r="B364" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="C364">
         <v>6150</v>
       </c>
     </row>
-    <row r="365" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A365">
+        <v>363</v>
+      </c>
       <c r="B365" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="C365">
         <v>6056</v>
       </c>
     </row>
-    <row r="366" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A366">
+        <v>364</v>
+      </c>
       <c r="B366" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="C366">
         <v>6018</v>
       </c>
     </row>
-    <row r="367" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A367">
+        <v>365</v>
+      </c>
       <c r="B367" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="C367">
         <v>6026</v>
       </c>
     </row>
-    <row r="368" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A368">
+        <v>366</v>
+      </c>
       <c r="B368" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="C368">
         <v>6112</v>
       </c>
     </row>
-    <row r="369" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A369">
+        <v>367</v>
+      </c>
       <c r="B369" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="C369">
         <v>6035</v>
       </c>
     </row>
-    <row r="370" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A370">
+        <v>368</v>
+      </c>
       <c r="B370" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C370">
         <v>6164</v>
       </c>
     </row>
-    <row r="371" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A371">
+        <v>369</v>
+      </c>
       <c r="B371" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C371">
         <v>6060</v>
       </c>
     </row>
-    <row r="372" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A372">
+        <v>370</v>
+      </c>
       <c r="B372" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="C372">
         <v>6208</v>

</xml_diff>